<commit_message>
initial loadout excel and f16 test
</commit_message>
<xml_diff>
--- a/FILES/OPBH Squad Load Out.xlsx
+++ b/FILES/OPBH Squad Load Out.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8cf75b30085b6be0/132nd/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\132nd\Mission Design\OPBH-Brief\FILES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="706" documentId="8_{12C9879F-218A-7F4D-A7D6-588CA3CB945F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FAEFBFA6-008F-452D-BECA-99D9494E6AC1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B91226B-4869-4EC3-9376-B29DDCC15256}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="2745" windowWidth="21600" windowHeight="15435" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5565" windowWidth="21600" windowHeight="15435" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="F-18C" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="84">
   <si>
     <t>Air to Air Weapons</t>
   </si>
@@ -277,6 +277,15 @@
   </si>
   <si>
     <t>Mk-82 AIR w/ ballute</t>
+  </si>
+  <si>
+    <t>AGM-84E</t>
+  </si>
+  <si>
+    <t>AAW-13 Datalink Pod</t>
+  </si>
+  <si>
+    <t>AN/AAQ-28 Lightning Pod</t>
   </si>
 </sst>
 </file>
@@ -826,13 +835,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>283547</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>93047</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>283907</xdr:colOff>
-      <xdr:row>49</xdr:row>
+      <xdr:row>51</xdr:row>
       <xdr:rowOff>93407</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing">
@@ -1540,10 +1549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521CF0D9-4AE3-4040-8D13-C9CB8923EC5B}">
-  <dimension ref="A1:W97"/>
+  <dimension ref="A1:W99"/>
   <sheetViews>
     <sheetView zoomScaleNormal="150" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2773,12 +2782,24 @@
     <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="27"/>
       <c r="B37" s="27"/>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="2"/>
+      <c r="C37" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D37" s="3">
+        <v>600000</v>
+      </c>
+      <c r="E37" s="2">
+        <v>627</v>
+      </c>
       <c r="F37" s="2"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="33"/>
+      <c r="G37" s="8">
+        <f>D37*F37</f>
+        <v>0</v>
+      </c>
+      <c r="H37" s="33">
+        <f>F37*E37</f>
+        <v>0</v>
+      </c>
       <c r="I37" s="28"/>
       <c r="J37" s="28"/>
       <c r="K37" s="28"/>
@@ -2797,24 +2818,12 @@
     <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="27"/>
       <c r="B38" s="27"/>
-      <c r="C38" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="3">
-        <v>58000</v>
-      </c>
-      <c r="E38" s="2">
-        <v>234</v>
-      </c>
+      <c r="C38" s="4"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="2"/>
       <c r="F38" s="2"/>
-      <c r="G38" s="8">
-        <f>D38*F38</f>
-        <v>0</v>
-      </c>
-      <c r="H38" s="33">
-        <f>F38*E38</f>
-        <v>0</v>
-      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="33"/>
       <c r="I38" s="28"/>
       <c r="J38" s="28"/>
       <c r="K38" s="28"/>
@@ -2834,7 +2843,7 @@
       <c r="A39" s="27"/>
       <c r="B39" s="27"/>
       <c r="C39" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D39" s="3">
         <v>58000</v>
@@ -2870,7 +2879,7 @@
       <c r="A40" s="27"/>
       <c r="B40" s="27"/>
       <c r="C40" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D40" s="3">
         <v>58000</v>
@@ -2906,12 +2915,12 @@
       <c r="A41" s="27"/>
       <c r="B41" s="27"/>
       <c r="C41" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D41" s="3">
         <v>58000</v>
       </c>
-      <c r="E41" s="18">
+      <c r="E41" s="2">
         <v>234</v>
       </c>
       <c r="F41" s="2"/>
@@ -2938,26 +2947,26 @@
       <c r="U41" s="27"/>
       <c r="V41" s="27"/>
     </row>
-    <row r="42" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="27"/>
       <c r="B42" s="27"/>
-      <c r="C42" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E42" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G42" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="H42" s="7" t="s">
-        <v>32</v>
+      <c r="C42" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D42" s="3">
+        <v>58000</v>
+      </c>
+      <c r="E42" s="18">
+        <v>234</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="8">
+        <f>D42*F42</f>
+        <v>0</v>
+      </c>
+      <c r="H42" s="33">
+        <f>F42*E42</f>
+        <v>0</v>
       </c>
       <c r="I42" s="28"/>
       <c r="J42" s="28"/>
@@ -2974,26 +2983,26 @@
       <c r="U42" s="27"/>
       <c r="V42" s="27"/>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="27"/>
       <c r="B43" s="27"/>
-      <c r="C43" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D43" s="3">
-        <v>1400000</v>
-      </c>
-      <c r="E43" s="2">
-        <v>300</v>
-      </c>
-      <c r="F43" s="2"/>
-      <c r="G43" s="8">
-        <f>D43*F43</f>
-        <v>0</v>
-      </c>
-      <c r="H43" s="9">
-        <f>F43*E43</f>
-        <v>0</v>
+      <c r="C43" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="I43" s="28"/>
       <c r="J43" s="28"/>
@@ -3013,21 +3022,21 @@
     <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="27"/>
       <c r="B44" s="27"/>
-      <c r="C44" s="19" t="s">
-        <v>40</v>
-      </c>
-      <c r="D44" s="16">
-        <v>5000</v>
-      </c>
-      <c r="E44" s="15">
-        <v>125</v>
-      </c>
-      <c r="F44" s="15"/>
-      <c r="G44" s="20">
+      <c r="C44" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D44" s="3">
+        <v>1400000</v>
+      </c>
+      <c r="E44" s="2">
+        <v>300</v>
+      </c>
+      <c r="F44" s="2"/>
+      <c r="G44" s="8">
         <f>D44*F44</f>
         <v>0</v>
       </c>
-      <c r="H44" s="21">
+      <c r="H44" s="9">
         <f>F44*E44</f>
         <v>0</v>
       </c>
@@ -3046,15 +3055,27 @@
       <c r="U44" s="27"/>
       <c r="V44" s="27"/>
     </row>
-    <row r="45" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="27"/>
       <c r="B45" s="27"/>
-      <c r="C45" s="28"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="28"/>
-      <c r="F45" s="29"/>
-      <c r="G45" s="29"/>
-      <c r="H45" s="29"/>
+      <c r="C45" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="D45" s="3">
+        <v>1300000</v>
+      </c>
+      <c r="E45" s="2">
+        <v>300</v>
+      </c>
+      <c r="F45" s="2"/>
+      <c r="G45" s="8">
+        <f>D45*F45</f>
+        <v>0</v>
+      </c>
+      <c r="H45" s="9">
+        <f>F45*E45</f>
+        <v>0</v>
+      </c>
       <c r="I45" s="28"/>
       <c r="J45" s="28"/>
       <c r="K45" s="28"/>
@@ -3070,21 +3091,25 @@
       <c r="U45" s="27"/>
       <c r="V45" s="27"/>
     </row>
-    <row r="46" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="27"/>
       <c r="B46" s="27"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="28"/>
-      <c r="F46" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G46" s="12">
-        <f>SUM(G4:G45)</f>
-        <v>0</v>
-      </c>
-      <c r="H46" s="13">
-        <f>SUM(H4:H45)</f>
+      <c r="C46" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="D46" s="16">
+        <v>5000</v>
+      </c>
+      <c r="E46" s="15">
+        <v>125</v>
+      </c>
+      <c r="F46" s="15"/>
+      <c r="G46" s="20">
+        <f>D46*F46</f>
+        <v>0</v>
+      </c>
+      <c r="H46" s="21">
+        <f>F46*E46</f>
         <v>0</v>
       </c>
       <c r="I46" s="28"/>
@@ -3108,9 +3133,9 @@
       <c r="C47" s="28"/>
       <c r="D47" s="28"/>
       <c r="E47" s="28"/>
-      <c r="F47" s="28"/>
-      <c r="G47" s="28"/>
-      <c r="H47" s="28"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
       <c r="I47" s="28"/>
       <c r="J47" s="28"/>
       <c r="K47" s="28"/>
@@ -3126,17 +3151,23 @@
       <c r="U47" s="27"/>
       <c r="V47" s="27"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="27"/>
       <c r="B48" s="27"/>
-      <c r="C48" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="D48" s="39"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="28"/>
-      <c r="G48" s="28"/>
-      <c r="H48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="G48" s="12">
+        <f>SUM(G4:G47)</f>
+        <v>0</v>
+      </c>
+      <c r="H48" s="13">
+        <f>SUM(H4:H47)</f>
+        <v>0</v>
+      </c>
       <c r="I48" s="28"/>
       <c r="J48" s="28"/>
       <c r="K48" s="28"/>
@@ -3155,11 +3186,9 @@
     <row r="49" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="27"/>
       <c r="B49" s="27"/>
-      <c r="C49" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D49" s="42"/>
-      <c r="E49" s="43"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
+      <c r="E49" s="28"/>
       <c r="F49" s="28"/>
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
@@ -3181,9 +3210,11 @@
     <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A50" s="27"/>
       <c r="B50" s="27"/>
-      <c r="C50" s="28"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="28"/>
+      <c r="C50" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="D50" s="39"/>
+      <c r="E50" s="40"/>
       <c r="F50" s="28"/>
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
@@ -3202,12 +3233,14 @@
       <c r="U50" s="27"/>
       <c r="V50" s="27"/>
     </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="27"/>
       <c r="B51" s="27"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
+      <c r="C51" s="41" t="s">
+        <v>46</v>
+      </c>
+      <c r="D51" s="42"/>
+      <c r="E51" s="43"/>
       <c r="F51" s="28"/>
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
@@ -3227,38 +3260,52 @@
       <c r="V51" s="27"/>
     </row>
     <row r="52" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-      <c r="F52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="L52" s="1"/>
-      <c r="M52" s="1"/>
-      <c r="N52" s="1"/>
-      <c r="O52" s="1"/>
-      <c r="P52" s="1"/>
-      <c r="Q52" s="1"/>
+      <c r="A52" s="27"/>
+      <c r="B52" s="27"/>
+      <c r="C52" s="28"/>
+      <c r="D52" s="28"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28"/>
+      <c r="G52" s="28"/>
+      <c r="H52" s="28"/>
+      <c r="I52" s="28"/>
+      <c r="J52" s="28"/>
+      <c r="K52" s="28"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="28"/>
+      <c r="O52" s="28"/>
+      <c r="P52" s="28"/>
+      <c r="Q52" s="28"/>
+      <c r="R52" s="27"/>
+      <c r="S52" s="27"/>
+      <c r="T52" s="27"/>
+      <c r="U52" s="27"/>
+      <c r="V52" s="27"/>
     </row>
     <row r="53" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-      <c r="F53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="L53" s="1"/>
-      <c r="M53" s="1"/>
-      <c r="N53" s="1"/>
-      <c r="O53" s="1"/>
-      <c r="P53" s="1"/>
-      <c r="Q53" s="1"/>
+      <c r="A53" s="27"/>
+      <c r="B53" s="27"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="28"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28"/>
+      <c r="G53" s="28"/>
+      <c r="H53" s="28"/>
+      <c r="I53" s="28"/>
+      <c r="J53" s="28"/>
+      <c r="K53" s="28"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="28"/>
+      <c r="O53" s="28"/>
+      <c r="P53" s="28"/>
+      <c r="Q53" s="28"/>
+      <c r="R53" s="27"/>
+      <c r="S53" s="27"/>
+      <c r="T53" s="27"/>
+      <c r="U53" s="27"/>
+      <c r="V53" s="27"/>
     </row>
     <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="C54" s="1"/>
@@ -3991,15 +4038,49 @@
       <c r="P96" s="1"/>
       <c r="Q96" s="1"/>
     </row>
-    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C97" s="1"/>
+      <c r="D97" s="1"/>
+      <c r="E97" s="1"/>
+      <c r="F97" s="1"/>
+      <c r="G97" s="1"/>
+      <c r="H97" s="1"/>
       <c r="I97" s="1"/>
+      <c r="J97" s="1"/>
+      <c r="K97" s="1"/>
+      <c r="L97" s="1"/>
+      <c r="M97" s="1"/>
+      <c r="N97" s="1"/>
+      <c r="O97" s="1"/>
+      <c r="P97" s="1"/>
+      <c r="Q97" s="1"/>
+    </row>
+    <row r="98" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C98" s="1"/>
+      <c r="D98" s="1"/>
+      <c r="E98" s="1"/>
+      <c r="F98" s="1"/>
+      <c r="G98" s="1"/>
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+      <c r="K98" s="1"/>
+      <c r="L98" s="1"/>
+      <c r="M98" s="1"/>
+      <c r="N98" s="1"/>
+      <c r="O98" s="1"/>
+      <c r="P98" s="1"/>
+      <c r="Q98" s="1"/>
+    </row>
+    <row r="99" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="I99" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C49:E49"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C51:E51"/>
   </mergeCells>
-  <conditionalFormatting sqref="G46">
+  <conditionalFormatting sqref="G48">
     <cfRule type="cellIs" dxfId="19" priority="3" operator="lessThanOrEqual">
       <formula>100000000</formula>
     </cfRule>
@@ -4010,7 +4091,7 @@
       <formula>100000000</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H46">
+  <conditionalFormatting sqref="H48">
     <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThanOrEqual">
       <formula>120000</formula>
     </cfRule>
@@ -4027,7 +4108,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7B99B8B-72E8-425C-B41A-ABCC4A5AD417}">
   <dimension ref="A1:V37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -5208,7 +5289,7 @@
   <dimension ref="A1:V46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C17"/>
+      <selection activeCell="K49" sqref="K49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6682,8 +6763,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FBC0FDA-2896-4052-9549-8CF0B0A42D52}">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>